<commit_message>
add antenna stick and add diagramm
</commit_message>
<xml_diff>
--- a/drafts/diagrams/угол и уровень.xlsx
+++ b/drafts/diagrams/угол и уровень.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin Pi Pi\Desktop\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\programms\dmitr_stantion_emu\drafts\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA522DB-088A-47D3-8593-F05118B3E716}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6492BAD6-CE90-42D4-8694-D27CB70B8B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,234 +180,444 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$37</c:f>
+              <c:f>Лист1!$A$2:$A$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="72"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="15">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="17">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="23">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>120</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>130</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="27">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>140</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="29">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>150</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="31">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>160</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="33">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>170</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="35">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="37">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>190</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="39">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="41">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="43">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="45">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="47">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="49">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="51">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="53">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="55">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="57">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="58">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="59">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="60">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="61">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="62">
                   <c:v>310</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="63">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="64">
                   <c:v>320</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="65">
+                  <c:v>325</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>330</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="67">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>340</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="69">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="70">
                   <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$37</c:f>
+              <c:f>Лист1!$B$4:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="70"/>
                 <c:pt idx="0">
-                  <c:v>-2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-3</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-3</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-3</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,7 +694,7 @@
         <c:axId val="469529000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-20"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1131,16 +1341,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1431,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,229 +1661,229 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>-2</v>
+      <c r="B2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>-5</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>-3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>-2</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>-4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1">
-        <v>-2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1">
-        <v>-5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1">
-        <v>-7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
-        <v>-6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1">
-        <v>-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1">
-        <v>-9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1">
-        <v>-8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1">
-        <v>-9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1">
-        <v>-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="B19" s="1">
-        <v>-6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="B20" s="1">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>190</v>
+        <v>95</v>
       </c>
       <c r="B21" s="1">
-        <v>-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B22" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="B23" s="1">
-        <v>-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="B24" s="1">
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>230</v>
+        <v>115</v>
       </c>
       <c r="B25" s="1">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="B26" s="1">
-        <v>-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="B27" s="1">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>260</v>
+        <v>130</v>
       </c>
       <c r="B28" s="1">
-        <v>-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="B29" s="1">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>280</v>
+        <v>140</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1681,62 +1891,351 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>290</v>
+        <v>145</v>
       </c>
       <c r="B31" s="1">
-        <v>-6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="B32" s="1">
-        <v>-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>310</v>
+        <v>155</v>
       </c>
       <c r="B33" s="1">
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>330</v>
+        <v>165</v>
       </c>
       <c r="B35" s="1">
-        <v>-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="B36" s="1">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
+        <v>175</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>180</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>185</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>190</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>195</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>200</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>205</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>210</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>215</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>220</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>225</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>230</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>235</v>
+      </c>
+      <c r="B49" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>240</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>245</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>250</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>255</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>260</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>265</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>270</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>275</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>280</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>285</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>290</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>295</v>
+      </c>
+      <c r="B61" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>300</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>305</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>310</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>315</v>
+      </c>
+      <c r="B65" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>320</v>
+      </c>
+      <c r="B66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>325</v>
+      </c>
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>330</v>
+      </c>
+      <c r="B68" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>335</v>
+      </c>
+      <c r="B69" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>340</v>
+      </c>
+      <c r="B70" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>345</v>
+      </c>
+      <c r="B71" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>350</v>
       </c>
-      <c r="B37" s="1">
-        <v>-3</v>
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>355</v>
+      </c>
+      <c r="B73" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>